<commit_message>
added handle for error documents
</commit_message>
<xml_diff>
--- a/tests/parsers/thermo_skanit/testdata/nan_columns_test.xlsx
+++ b/tests/parsers/thermo_skanit/testdata/nan_columns_test.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,7 +442,6 @@
       <c r="J1" t="inlineStr"/>
       <c r="K1" t="inlineStr"/>
       <c r="L1" t="inlineStr"/>
-      <c r="M1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -461,7 +460,6 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -480,7 +478,6 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -495,7 +492,6 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -514,7 +510,6 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -533,13 +528,16 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>MISSED</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
@@ -548,7 +546,6 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -559,7 +556,11 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>MISSED</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
@@ -567,7 +568,6 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -582,7 +582,6 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -617,7 +616,6 @@
       <c r="L10" t="n">
         <v>8</v>
       </c>
-      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -625,9 +623,7 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>1.7455</v>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
         <v>1.6148</v>
       </c>
@@ -652,7 +648,6 @@
       <c r="L11" t="n">
         <v>0.0761</v>
       </c>
-      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -663,8 +658,10 @@
       <c r="B12" t="n">
         <v>1.3625</v>
       </c>
-      <c r="C12" t="n">
-        <v>1.1336</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MISSED</t>
+        </is>
       </c>
       <c r="D12" t="n">
         <v>0.3925</v>
@@ -687,7 +684,6 @@
       <c r="L12" t="n">
         <v>0.2635</v>
       </c>
-      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -702,7 +698,6 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -737,7 +732,6 @@
       <c r="L14" t="n">
         <v>8</v>
       </c>
-      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -788,7 +782,6 @@
           <t>Un0004</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -839,7 +832,6 @@
           <t>Un0015</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -847,6 +839,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>General information</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Report generated with SW version</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SkanIt Software 7.0 RE for Microplate Readers RE, ver. 7.0.0.50</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -863,7 +907,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>General information</t>
+          <t>Session information</t>
         </is>
       </c>
       <c r="B1" t="inlineStr"/>
@@ -880,65 +924,6 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Report generated with SW version</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>SkanIt Software 7.0 RE for Microplate Readers RE, ver. 7.0.0.50</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Session information</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-      <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
           <t>Session notes</t>
@@ -966,13 +951,6 @@
           <t>6/5/2023 6:09:56 PM</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -980,80 +958,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Instrument information</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-      <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Varioskan LUX</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Serial number</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>3020-81776</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1070,7 +974,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Layout definitions</t>
+          <t>Instrument information</t>
         </is>
       </c>
       <c r="B1" t="inlineStr"/>
@@ -1086,26 +990,77 @@
       <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Plate template</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>96 Well Microplate</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Varioskan LUX</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Serial number</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3020-81776</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Layout definitions</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Plate template</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>96 Well Microplate</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>